<commit_message>
Risk assessment and timesheet update
</commit_message>
<xml_diff>
--- a/Admin/ganges_timesheet.xlsx
+++ b/Admin/ganges_timesheet.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\2nd Year\D4\D4-Ganges\Admin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohammed\Documents\2nd year\Semester 2\Electronic design\D4-Ganges\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -366,15 +366,15 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
@@ -383,7 +383,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -400,7 +400,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>42789</v>
       </c>
@@ -420,7 +420,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>42790</v>
       </c>
@@ -436,8 +436,11 @@
       <c r="E4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>42791</v>
       </c>
@@ -450,8 +453,11 @@
       <c r="E5">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>42792</v>
       </c>
@@ -467,8 +473,11 @@
       <c r="E6">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>42793</v>
       </c>
@@ -478,128 +487,143 @@
       <c r="E7">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>42794</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>42795</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>42796</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>42797</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>42798</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>42799</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>42800</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>42801</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>42802</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>42803</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>42804</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>42805</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>42806</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>42807</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>42808</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>42809</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>42810</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>42811</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>42812</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>42813</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>42814</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>42815</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>42816</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>42817</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>42818</v>
       </c>

</xml_diff>

<commit_message>
Drone code for receiving pot values, sending telemetry and updated timesheet
test1 for drone receives potentiometer values. test3 receives
potentiometer values and sends telemetry back at 1/s (intermittent).
test3 also successfully implements encryption and decryption for both
directions.
Also updated timesheet.
</commit_message>
<xml_diff>
--- a/Admin/ganges_timesheet.xlsx
+++ b/Admin/ganges_timesheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\2nd Year\D4\D4-Ganges\Admin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\D4\D4-Ganges\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -79,10 +79,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -176,6 +176,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -211,6 +228,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -366,7 +400,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -375,13 +409,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -401,7 +435,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>42789</v>
       </c>
       <c r="B3">
@@ -421,7 +455,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>42790</v>
       </c>
       <c r="B4">
@@ -441,7 +475,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>42791</v>
       </c>
       <c r="B5">
@@ -458,7 +492,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>42792</v>
       </c>
       <c r="B6">
@@ -478,7 +512,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>42793</v>
       </c>
       <c r="B7">
@@ -495,7 +529,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>42794</v>
       </c>
       <c r="B8">
@@ -512,7 +546,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>42795</v>
       </c>
       <c r="B9">
@@ -529,126 +563,153 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>42796</v>
       </c>
       <c r="B10">
         <v>7</v>
       </c>
+      <c r="C10">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>42797</v>
       </c>
       <c r="B11">
         <v>6</v>
       </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>42798</v>
       </c>
       <c r="B12">
         <v>6</v>
       </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>42799</v>
       </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>42800</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>42801</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>42802</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>42803</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>42804</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>42805</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>42806</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>42807</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>42808</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>42809</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>42810</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>42811</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>42812</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <v>42813</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <v>42814</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="A29" s="1">
         <v>42815</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>42816</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="A31" s="1">
         <v>42817</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <v>42818</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reuploaded comms and updated timesheet
Reuploaded comms and updated timesheet
</commit_message>
<xml_diff>
--- a/Admin/ganges_timesheet.xlsx
+++ b/Admin/ganges_timesheet.xlsx
@@ -400,7 +400,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,15 +622,24 @@
       <c r="A14" s="1">
         <v>42800</v>
       </c>
+      <c r="E14">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>42801</v>
       </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>42802</v>
+      </c>
+      <c r="E16">
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>